<commit_message>
Commiting last changes from friday. No nice curves yet.
</commit_message>
<xml_diff>
--- a/dpr-data_edited.xlsx
+++ b/dpr-data_edited.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Per\Dropbox\Pers dropbox\F\Projektarbete15\oil\Matlab Project Shale Oil\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Per\Documents\GitHub\matlabTightOil\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1385,10 +1385,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -1533,7 +1534,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1558,6 +1559,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -9798,10 +9800,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:L108"/>
+  <dimension ref="A1:N108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J107" sqref="J107"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B106" sqref="B3:B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9817,7 +9819,7 @@
     <col min="10" max="10" width="10.7109375" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>436</v>
       </c>
@@ -9834,7 +9836,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="13"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -9860,7 +9862,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>39083</v>
       </c>
@@ -9886,19 +9888,17 @@
         <v>1599345.8389999999</v>
       </c>
       <c r="J3" s="14">
-        <f>L3/B3</f>
+        <f>C3/B3</f>
         <v>0.81920848856033868</v>
       </c>
-      <c r="K3" s="14">
-        <f>C3</f>
-        <v>42</v>
-      </c>
-      <c r="L3" s="14">
-        <f t="shared" ref="L3:L20" si="0">K3</f>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="N3" s="18">
+        <f>J3*0.8</f>
+        <v>0.65536679084827099</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>39114</v>
       </c>
@@ -9924,19 +9924,17 @@
         <v>1651068.6429999999</v>
       </c>
       <c r="J4" s="14">
-        <f>L4/B3</f>
-        <v>0.79970352454699722</v>
-      </c>
-      <c r="K4" s="14">
-        <f t="shared" ref="K4:K67" si="1">C4</f>
-        <v>41</v>
-      </c>
-      <c r="L4" s="14">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ref="J4:J67" si="0">C4/B4</f>
+        <v>0.73437220132545233</v>
+      </c>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="N4" s="18">
+        <f t="shared" ref="N4:N67" si="1">J4*0.8</f>
+        <v>0.58749776106036189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>39142</v>
       </c>
@@ -9962,19 +9960,17 @@
         <v>1657528.8060000001</v>
       </c>
       <c r="J5" s="14">
-        <f>L5/B3</f>
-        <v>0.78019856053365588</v>
-      </c>
-      <c r="K5" s="14">
+        <f t="shared" si="0"/>
+        <v>0.68461498964519829</v>
+      </c>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="N5" s="18">
         <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="L5" s="14">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.54769199171615868</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>39173</v>
       </c>
@@ -10000,19 +9996,17 @@
         <v>1669597.933</v>
       </c>
       <c r="J6" s="14">
-        <f t="shared" ref="J6:J11" si="2">L6/B4</f>
-        <v>0.68063765000895582</v>
-      </c>
-      <c r="K6" s="14">
+        <f t="shared" si="0"/>
+        <v>0.68357618276668464</v>
+      </c>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="N6" s="18">
         <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="L6" s="14">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.54686094621334769</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>39203</v>
       </c>
@@ -10038,19 +10032,17 @@
         <v>1634170.0970000001</v>
       </c>
       <c r="J7" s="14">
-        <f t="shared" si="2"/>
-        <v>0.63326886542180838</v>
-      </c>
-      <c r="K7" s="14">
+        <f t="shared" si="0"/>
+        <v>0.67445633350954259</v>
+      </c>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="N7" s="18">
         <f t="shared" si="1"/>
-        <v>37</v>
-      </c>
-      <c r="L7" s="14">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.53956506680763405</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>39234</v>
       </c>
@@ -10076,19 +10068,17 @@
         <v>1654730.9669999999</v>
       </c>
       <c r="J8" s="14">
-        <f>L8/B6</f>
-        <v>0.64759848893685912</v>
-      </c>
-      <c r="K8" s="14">
+        <f t="shared" si="0"/>
+        <v>0.59505115787037799</v>
+      </c>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="N8" s="18">
         <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
-      <c r="L8" s="14">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.4760409262963024</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>39264</v>
       </c>
@@ -10114,19 +10104,17 @@
         <v>1651882.581</v>
       </c>
       <c r="J9" s="14">
-        <f t="shared" ref="J9:J72" si="3">L9/B7</f>
-        <v>0.63799923440091866</v>
-      </c>
-      <c r="K9" s="14">
+        <f t="shared" si="0"/>
+        <v>0.55936456185772965</v>
+      </c>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="N9" s="18">
         <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="L9" s="14">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.44749164948618375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>39295</v>
       </c>
@@ -10152,19 +10140,17 @@
         <v>1640219.8060000001</v>
       </c>
       <c r="J10" s="14">
-        <f t="shared" si="3"/>
-        <v>0.5454635613811798</v>
-      </c>
-      <c r="K10" s="14">
+        <f t="shared" si="0"/>
+        <v>0.54595086442220198</v>
+      </c>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="N10" s="18">
         <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="L10" s="14">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.43676069153776159</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>39326</v>
       </c>
@@ -10190,19 +10176,17 @@
         <v>1648026.8330000001</v>
       </c>
       <c r="J11" s="14">
-        <f t="shared" si="3"/>
-        <v>0.51141902798420991</v>
-      </c>
-      <c r="K11" s="14">
+        <f t="shared" si="0"/>
+        <v>0.53264976613346204</v>
+      </c>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="N11" s="18">
         <f t="shared" si="1"/>
-        <v>32</v>
-      </c>
-      <c r="L11" s="14">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.42611981290676965</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>39356</v>
       </c>
@@ -10228,19 +10212,17 @@
         <v>1643920.9029999999</v>
       </c>
       <c r="J12" s="14">
-        <f t="shared" si="3"/>
-        <v>0.49631896765654726</v>
-      </c>
-      <c r="K12" s="14">
+        <f t="shared" si="0"/>
+        <v>0.56661504174064148</v>
+      </c>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="N12" s="18">
         <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="L12" s="14">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.45329203339251323</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>39387</v>
       </c>
@@ -10266,19 +10248,17 @@
         <v>1652223.267</v>
       </c>
       <c r="J13" s="14">
-        <f t="shared" si="3"/>
-        <v>0.49935915575012069</v>
-      </c>
-      <c r="K13" s="14">
+        <f t="shared" si="0"/>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="N13" s="18">
         <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="L13" s="14">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.42666666666666669</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>39417</v>
       </c>
@@ -10304,19 +10284,17 @@
         <v>1644426.0649999999</v>
       </c>
       <c r="J14" s="14">
-        <f t="shared" si="3"/>
-        <v>0.56661504174064148</v>
-      </c>
-      <c r="K14" s="14">
+        <f t="shared" si="0"/>
+        <v>0.51847499222287508</v>
+      </c>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="N14" s="18">
         <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="L14" s="14">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.4147799937783001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>39448</v>
       </c>
@@ -10342,19 +10320,17 @@
         <v>1645492.0970000001</v>
       </c>
       <c r="J15" s="14">
-        <f t="shared" si="3"/>
-        <v>0.55111111111111111</v>
-      </c>
-      <c r="K15" s="14">
+        <f t="shared" si="0"/>
+        <v>0.5666343746001572</v>
+      </c>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="N15" s="18">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="L15" s="14">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.45330749968012579</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>39479</v>
       </c>
@@ -10380,19 +10356,17 @@
         <v>1648505.138</v>
       </c>
       <c r="J16" s="14">
-        <f t="shared" si="3"/>
-        <v>0.53575749196363764</v>
-      </c>
-      <c r="K16" s="14">
+        <f t="shared" si="0"/>
+        <v>0.63795196839050883</v>
+      </c>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="N16" s="18">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="L16" s="14">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.51036157471240706</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>39508</v>
       </c>
@@ -10418,19 +10392,17 @@
         <v>1664576.581</v>
       </c>
       <c r="J17" s="14">
-        <f t="shared" si="3"/>
-        <v>0.54835584638724888</v>
-      </c>
-      <c r="K17" s="14">
+        <f t="shared" si="0"/>
+        <v>0.49794184039304212</v>
+      </c>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="N17" s="18">
         <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="L17" s="14">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.39835347231443374</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>39539</v>
       </c>
@@ -10456,19 +10428,17 @@
         <v>1646640.0330000001</v>
       </c>
       <c r="J18" s="14">
-        <f t="shared" si="3"/>
-        <v>0.63795196839050883</v>
-      </c>
-      <c r="K18" s="14">
+        <f t="shared" si="0"/>
+        <v>0.46001572957010789</v>
+      </c>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="N18" s="18">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="L18" s="14">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.36801258365608636</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>39569</v>
       </c>
@@ -10494,19 +10464,17 @@
         <v>1660219.6129999999</v>
       </c>
       <c r="J19" s="14">
-        <f t="shared" si="3"/>
-        <v>0.53113796308591155</v>
-      </c>
-      <c r="K19" s="14">
+        <f t="shared" si="0"/>
+        <v>0.44984887889224712</v>
+      </c>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="N19" s="18">
         <f t="shared" si="1"/>
-        <v>32</v>
-      </c>
-      <c r="L19" s="14">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.35987910311379773</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>39600</v>
       </c>
@@ -10532,19 +10500,17 @@
         <v>1687947.2</v>
       </c>
       <c r="J20" s="14">
-        <f t="shared" si="3"/>
-        <v>0.50453338081882804</v>
-      </c>
-      <c r="K20" s="14">
+        <f t="shared" si="0"/>
+        <v>0.53071099664403343</v>
+      </c>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="N20" s="18">
         <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="L20" s="14">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.42456879731522679</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>39630</v>
       </c>
@@ -10570,19 +10536,17 @@
         <v>1683461.129</v>
       </c>
       <c r="J21" s="14">
-        <f t="shared" si="3"/>
-        <v>0.49202221128839529</v>
-      </c>
-      <c r="K21" s="14">
+        <f t="shared" si="0"/>
+        <v>0.54702885186458694</v>
+      </c>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="N21" s="18">
         <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="L21" s="14">
-        <f>K21</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.43762308149166956</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>39661</v>
       </c>
@@ -10608,19 +10572,17 @@
         <v>1660041.9350000001</v>
       </c>
       <c r="J22" s="14">
-        <f t="shared" si="3"/>
-        <v>0.43705611488332163</v>
-      </c>
-      <c r="K22" s="14">
+        <f t="shared" si="0"/>
+        <v>0.51277543366150957</v>
+      </c>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="N22" s="18">
         <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="L22" s="14">
-        <f>K22*0.8</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.41022034692920767</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>39692</v>
       </c>
@@ -10646,19 +10608,17 @@
         <v>1570086.733</v>
       </c>
       <c r="J23" s="14">
-        <f t="shared" si="3"/>
-        <v>0.42511956487762187</v>
-      </c>
-      <c r="K23" s="14">
+        <f t="shared" si="0"/>
+        <v>0.50910397700047916</v>
+      </c>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="N23" s="18">
         <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="L23" s="14">
-        <f t="shared" ref="L23:L59" si="4">K23*0.8</f>
-        <v>27.200000000000003</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.40728318160038335</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>39722</v>
       </c>
@@ -10684,19 +10644,17 @@
         <v>1682555.5160000001</v>
       </c>
       <c r="J24" s="14">
-        <f t="shared" si="3"/>
-        <v>0.38677918424753871</v>
-      </c>
-      <c r="K24" s="14">
+        <f t="shared" si="0"/>
+        <v>0.45306021582141193</v>
+      </c>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="N24" s="18">
         <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="L24" s="14">
-        <f t="shared" si="4"/>
-        <v>26.400000000000002</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.36244817265712959</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>39753</v>
       </c>
@@ -10722,19 +10680,17 @@
         <v>1694299.9669999999</v>
       </c>
       <c r="J25" s="14">
-        <f t="shared" si="3"/>
-        <v>0.39530426449448969</v>
-      </c>
-      <c r="K25" s="14">
+        <f t="shared" si="0"/>
+        <v>0.45577592398210048</v>
+      </c>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="N25" s="18">
         <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="L25" s="14">
-        <f t="shared" si="4"/>
-        <v>26.400000000000002</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.36462073918568039</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>39783</v>
       </c>
@@ -10760,19 +10716,17 @@
         <v>1690372.226</v>
       </c>
       <c r="J26" s="14">
-        <f t="shared" si="3"/>
-        <v>0.36244817265712959</v>
-      </c>
-      <c r="K26" s="14">
+        <f t="shared" si="0"/>
+        <v>0.53125553391181157</v>
+      </c>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="N26" s="18">
         <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="L26" s="14">
-        <f t="shared" si="4"/>
-        <v>26.400000000000002</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.4250044271294493</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>39814</v>
       </c>
@@ -10798,19 +10752,17 @@
         <v>1718324.3230000001</v>
       </c>
       <c r="J27" s="14">
-        <f t="shared" si="3"/>
-        <v>0.36462073918568039</v>
-      </c>
-      <c r="K27" s="14">
+        <f t="shared" si="0"/>
+        <v>0.71459506279774798</v>
+      </c>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="N27" s="18">
         <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="L27" s="14">
-        <f t="shared" si="4"/>
-        <v>26.400000000000002</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.57167605023819845</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>39845</v>
       </c>
@@ -10836,19 +10788,17 @@
         <v>1704801.9639999999</v>
       </c>
       <c r="J28" s="14">
-        <f t="shared" si="3"/>
-        <v>0.4250044271294493</v>
-      </c>
-      <c r="K28" s="14">
+        <f t="shared" si="0"/>
+        <v>0.84693563289190021</v>
+      </c>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="N28" s="18">
         <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="L28" s="14">
-        <f t="shared" si="4"/>
-        <v>26.400000000000002</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.67754850631352026</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>39873</v>
       </c>
@@ -10874,19 +10824,17 @@
         <v>1682055.1939999999</v>
       </c>
       <c r="J29" s="14">
-        <f t="shared" si="3"/>
-        <v>0.57167605023819845</v>
-      </c>
-      <c r="K29" s="14">
+        <f t="shared" si="0"/>
+        <v>0.89153046062407126</v>
+      </c>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="N29" s="18">
         <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="L29" s="14">
-        <f t="shared" si="4"/>
-        <v>26.400000000000002</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.71322436849925708</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>39904</v>
       </c>
@@ -10912,19 +10860,17 @@
         <v>1653524.1669999999</v>
       </c>
       <c r="J30" s="14">
-        <f t="shared" si="3"/>
-        <v>0.6980802792321118</v>
-      </c>
-      <c r="K30" s="14">
+        <f t="shared" si="0"/>
+        <v>0.9079499025289075</v>
+      </c>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="N30" s="18">
         <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="L30" s="14">
-        <f t="shared" si="4"/>
-        <v>27.200000000000003</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.72635992202312605</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>39934</v>
       </c>
@@ -10950,19 +10896,17 @@
         <v>1616026.5160000001</v>
       </c>
       <c r="J31" s="14">
-        <f t="shared" si="3"/>
-        <v>0.75645008780224232</v>
-      </c>
-      <c r="K31" s="14">
+        <f t="shared" si="0"/>
+        <v>1.0805137070881699</v>
+      </c>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="N31" s="18">
         <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="L31" s="14">
-        <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.86441096567053588</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>39965</v>
       </c>
@@ -10988,19 +10932,17 @@
         <v>1590866.1329999999</v>
       </c>
       <c r="J32" s="14">
-        <f t="shared" si="3"/>
-        <v>0.8331775576147622</v>
-      </c>
-      <c r="K32" s="14">
+        <f t="shared" si="0"/>
+        <v>1.3002600520104022</v>
+      </c>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="N32" s="18">
         <f t="shared" si="1"/>
-        <v>39</v>
-      </c>
-      <c r="L32" s="14">
-        <f t="shared" si="4"/>
-        <v>31.200000000000003</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.0402080416083217</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>39995</v>
       </c>
@@ -11026,19 +10968,17 @@
         <v>1588072.9029999999</v>
       </c>
       <c r="J33" s="14">
-        <f t="shared" si="3"/>
-        <v>1.0619906149666583</v>
-      </c>
-      <c r="K33" s="14">
+        <f t="shared" si="0"/>
+        <v>1.2806766738146296</v>
+      </c>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="N33" s="18">
         <f t="shared" si="1"/>
-        <v>43</v>
-      </c>
-      <c r="L33" s="14">
-        <f t="shared" si="4"/>
-        <v>34.4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.0245413390517037</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>40026</v>
       </c>
@@ -11064,19 +11004,17 @@
         <v>1571233.774</v>
       </c>
       <c r="J34" s="14">
-        <f t="shared" si="3"/>
-        <v>1.2535840501433622</v>
-      </c>
-      <c r="K34" s="14">
+        <f t="shared" si="0"/>
+        <v>1.2059631026608164</v>
+      </c>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="N34" s="18">
         <f t="shared" si="1"/>
-        <v>47</v>
-      </c>
-      <c r="L34" s="14">
-        <f t="shared" si="4"/>
-        <v>37.6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.96477048212865313</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>40057</v>
       </c>
@@ -11102,19 +11040,17 @@
         <v>1532562.067</v>
       </c>
       <c r="J35" s="14">
-        <f t="shared" si="3"/>
-        <v>1.2151536812008579</v>
-      </c>
-      <c r="K35" s="14">
+        <f t="shared" si="0"/>
+        <v>1.1045176939403127</v>
+      </c>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="N35" s="18">
         <f t="shared" si="1"/>
-        <v>51</v>
-      </c>
-      <c r="L35" s="14">
-        <f t="shared" si="4"/>
-        <v>40.800000000000004</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.88361415515225028</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>40087</v>
       </c>
@@ -11140,19 +11076,17 @@
         <v>1526340.4839999999</v>
       </c>
       <c r="J36" s="14">
-        <f t="shared" si="3"/>
-        <v>1.1084597028712186</v>
-      </c>
-      <c r="K36" s="14">
+        <f t="shared" si="0"/>
+        <v>1.2493348448742567</v>
+      </c>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="N36" s="18">
         <f t="shared" si="1"/>
-        <v>54</v>
-      </c>
-      <c r="L36" s="14">
-        <f t="shared" si="4"/>
-        <v>43.2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.99946787589940544</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>40118</v>
       </c>
@@ -11178,19 +11112,17 @@
         <v>1591080.1329999999</v>
       </c>
       <c r="J37" s="14">
-        <f t="shared" si="3"/>
-        <v>1.0048945293888336</v>
-      </c>
-      <c r="K37" s="14">
+        <f t="shared" si="0"/>
+        <v>1.2684249661024363</v>
+      </c>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="N37" s="18">
         <f t="shared" si="1"/>
-        <v>58</v>
-      </c>
-      <c r="L37" s="14">
-        <f>K37*0.8</f>
-        <v>46.400000000000006</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.0147399728819491</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>40148</v>
       </c>
@@ -11216,19 +11148,17 @@
         <v>1613883</v>
       </c>
       <c r="J38" s="14">
-        <f t="shared" si="3"/>
-        <v>1.1845545195844807</v>
-      </c>
-      <c r="K38" s="14">
+        <f t="shared" si="0"/>
+        <v>1.0244589576130105</v>
+      </c>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="N38" s="18">
         <f t="shared" si="1"/>
-        <v>64</v>
-      </c>
-      <c r="L38" s="14">
-        <f t="shared" si="4"/>
-        <v>51.2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.81956716609040847</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>40179</v>
       </c>
@@ -11254,19 +11184,17 @@
         <v>1696671.4839999999</v>
       </c>
       <c r="J39" s="14">
-        <f t="shared" si="3"/>
-        <v>1.2246861741678694</v>
-      </c>
-      <c r="K39" s="14">
+        <f t="shared" si="0"/>
+        <v>1.0904106174839554</v>
+      </c>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="N39" s="18">
         <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="L39" s="14">
-        <f t="shared" si="4"/>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.87232849398716439</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>40210</v>
       </c>
@@ -11292,19 +11220,17 @@
         <v>1755244.2860000001</v>
       </c>
       <c r="J40" s="14">
-        <f t="shared" si="3"/>
-        <v>0.98604174670252276</v>
-      </c>
-      <c r="K40" s="14">
+        <f t="shared" si="0"/>
+        <v>1.0153221340225218</v>
+      </c>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="N40" s="18">
         <f t="shared" si="1"/>
-        <v>77</v>
-      </c>
-      <c r="L40" s="14">
-        <f t="shared" si="4"/>
-        <v>61.6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.81225770721801749</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>40238</v>
       </c>
@@ -11330,19 +11256,17 @@
         <v>1752976.3230000001</v>
       </c>
       <c r="J41" s="14">
-        <f t="shared" si="3"/>
-        <v>1.0094086858994329</v>
-      </c>
-      <c r="K41" s="14">
+        <f t="shared" si="0"/>
+        <v>0.90752235193940878</v>
+      </c>
+      <c r="K41" s="14"/>
+      <c r="L41" s="14"/>
+      <c r="N41" s="18">
         <f t="shared" si="1"/>
-        <v>81</v>
-      </c>
-      <c r="L41" s="14">
-        <f t="shared" si="4"/>
-        <v>64.8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.72601788155152702</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>40269</v>
       </c>
@@ -11368,19 +11292,17 @@
         <v>1734715.6669999999</v>
       </c>
       <c r="J42" s="14">
-        <f t="shared" si="3"/>
-        <v>0.90719691974999339</v>
-      </c>
-      <c r="K42" s="14">
+        <f t="shared" si="0"/>
+        <v>0.89765669850216578</v>
+      </c>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="N42" s="18">
         <f t="shared" si="1"/>
-        <v>86</v>
-      </c>
-      <c r="L42" s="14">
-        <f t="shared" si="4"/>
-        <v>68.8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.71812535880173267</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>40299</v>
       </c>
@@ -11406,19 +11328,17 @@
         <v>1814277.226</v>
       </c>
       <c r="J43" s="14">
-        <f t="shared" si="3"/>
-        <v>0.8066865350572523</v>
-      </c>
-      <c r="K43" s="14">
+        <f t="shared" si="0"/>
+        <v>0.92282137254298813</v>
+      </c>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
+      <c r="N43" s="18">
         <f t="shared" si="1"/>
-        <v>90</v>
-      </c>
-      <c r="L43" s="14">
-        <f t="shared" si="4"/>
-        <v>72</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.73825709803439055</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>40330</v>
       </c>
@@ -11444,19 +11364,17 @@
         <v>1850705.9669999999</v>
       </c>
       <c r="J44" s="14">
-        <f t="shared" si="3"/>
-        <v>0.80162830749960867</v>
-      </c>
-      <c r="K44" s="14">
+        <f t="shared" si="0"/>
+        <v>0.9201571935205598</v>
+      </c>
+      <c r="K44" s="14"/>
+      <c r="L44" s="14"/>
+      <c r="N44" s="18">
         <f t="shared" si="1"/>
-        <v>96</v>
-      </c>
-      <c r="L44" s="14">
-        <f t="shared" si="4"/>
-        <v>76.800000000000011</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.73612575481644793</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>40360</v>
       </c>
@@ -11482,19 +11400,17 @@
         <v>1836462.0649999999</v>
       </c>
       <c r="J45" s="14">
-        <f t="shared" si="3"/>
-        <v>0.83669137777230929</v>
-      </c>
-      <c r="K45" s="14">
+        <f t="shared" si="0"/>
+        <v>0.85751036158353577</v>
+      </c>
+      <c r="K45" s="14"/>
+      <c r="L45" s="14"/>
+      <c r="N45" s="18">
         <f t="shared" si="1"/>
-        <v>102</v>
-      </c>
-      <c r="L45" s="14">
-        <f t="shared" si="4"/>
-        <v>81.600000000000009</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.68600828926682866</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>40391</v>
       </c>
@@ -11520,19 +11436,17 @@
         <v>1858522.8389999999</v>
       </c>
       <c r="J46" s="14">
-        <f t="shared" si="3"/>
-        <v>0.84347742739384646</v>
-      </c>
-      <c r="K46" s="14">
+        <f t="shared" si="0"/>
+        <v>0.83836351441985246</v>
+      </c>
+      <c r="K46" s="14"/>
+      <c r="L46" s="14"/>
+      <c r="N46" s="18">
         <f t="shared" si="1"/>
-        <v>110</v>
-      </c>
-      <c r="L46" s="14">
-        <f t="shared" si="4"/>
-        <v>88</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.67069081153588206</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>40422</v>
       </c>
@@ -11558,19 +11472,17 @@
         <v>1895522.6</v>
       </c>
       <c r="J47" s="14">
-        <f t="shared" si="3"/>
-        <v>0.80034300414463344</v>
-      </c>
-      <c r="K47" s="14">
+        <f t="shared" si="0"/>
+        <v>0.84890249035175946</v>
+      </c>
+      <c r="K47" s="14"/>
+      <c r="L47" s="14"/>
+      <c r="N47" s="18">
         <f t="shared" si="1"/>
-        <v>119</v>
-      </c>
-      <c r="L47" s="14">
-        <f t="shared" si="4"/>
-        <v>95.2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.67912199228140757</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>40452</v>
       </c>
@@ -11596,19 +11508,17 @@
         <v>1954265.9029999999</v>
       </c>
       <c r="J48" s="14">
-        <f t="shared" si="3"/>
-        <v>0.78653740625571611</v>
-      </c>
-      <c r="K48" s="14">
+        <f t="shared" si="0"/>
+        <v>0.86804971435108236</v>
+      </c>
+      <c r="K48" s="14"/>
+      <c r="L48" s="14"/>
+      <c r="N48" s="18">
         <f t="shared" si="1"/>
-        <v>129</v>
-      </c>
-      <c r="L48" s="14">
-        <f>K48*0.8</f>
-        <v>103.2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.69443977148086589</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>40483</v>
       </c>
@@ -11634,19 +11544,17 @@
         <v>2044164.3330000001</v>
       </c>
       <c r="J49" s="14">
-        <f t="shared" si="3"/>
-        <v>0.78755323474650629</v>
-      </c>
-      <c r="K49" s="14">
+        <f t="shared" si="0"/>
+        <v>0.95485870858819299</v>
+      </c>
+      <c r="K49" s="14"/>
+      <c r="L49" s="14"/>
+      <c r="N49" s="18">
         <f t="shared" si="1"/>
-        <v>138</v>
-      </c>
-      <c r="L49" s="14">
-        <f t="shared" si="4"/>
-        <v>110.4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.76388696687055446</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>40513</v>
       </c>
@@ -11672,19 +11580,17 @@
         <v>2184989.29</v>
       </c>
       <c r="J50" s="14">
-        <f t="shared" si="3"/>
-        <v>0.79672159828812517</v>
-      </c>
-      <c r="K50" s="14">
+        <f t="shared" si="0"/>
+        <v>1.0360808143035156</v>
+      </c>
+      <c r="K50" s="14"/>
+      <c r="L50" s="14"/>
+      <c r="N50" s="18">
         <f t="shared" si="1"/>
-        <v>148</v>
-      </c>
-      <c r="L50" s="14">
-        <f t="shared" si="4"/>
-        <v>118.4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.82886465144281252</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>40544</v>
       </c>
@@ -11710,19 +11616,17 @@
         <v>2225429.7420000001</v>
       </c>
       <c r="J51" s="14">
-        <f t="shared" si="3"/>
-        <v>0.88013063574216044</v>
-      </c>
-      <c r="K51" s="14">
+        <f t="shared" si="0"/>
+        <v>1.1705636374344779</v>
+      </c>
+      <c r="K51" s="14"/>
+      <c r="L51" s="14"/>
+      <c r="N51" s="18">
         <f t="shared" si="1"/>
-        <v>159</v>
-      </c>
-      <c r="L51" s="14">
-        <f t="shared" si="4"/>
-        <v>127.2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.9364509099475824</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>40575</v>
       </c>
@@ -11748,19 +11652,17 @@
         <v>2242511.071</v>
       </c>
       <c r="J52" s="14">
-        <f t="shared" si="3"/>
-        <v>0.96327513546056587</v>
-      </c>
-      <c r="K52" s="14">
+        <f t="shared" si="0"/>
+        <v>1.0990415335463259</v>
+      </c>
+      <c r="K52" s="14"/>
+      <c r="L52" s="14"/>
+      <c r="N52" s="18">
         <f t="shared" si="1"/>
-        <v>172</v>
-      </c>
-      <c r="L52" s="14">
-        <f t="shared" si="4"/>
-        <v>137.6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.87923322683706084</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>40603</v>
       </c>
@@ -11786,19 +11688,17 @@
         <v>2323930.9029999999</v>
       </c>
       <c r="J53" s="14">
-        <f t="shared" si="3"/>
-        <v>1.0836916190588375</v>
-      </c>
-      <c r="K53" s="14">
+        <f t="shared" si="0"/>
+        <v>1.1701112877583466</v>
+      </c>
+      <c r="K53" s="14"/>
+      <c r="L53" s="14"/>
+      <c r="N53" s="18">
         <f t="shared" si="1"/>
-        <v>184</v>
-      </c>
-      <c r="L53" s="14">
-        <f t="shared" si="4"/>
-        <v>147.20000000000002</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.93608903020667733</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>40634</v>
       </c>
@@ -11824,19 +11724,17 @@
         <v>2424514.7999999998</v>
       </c>
       <c r="J54" s="14">
-        <f t="shared" si="3"/>
-        <v>0.99680511182108622</v>
-      </c>
-      <c r="K54" s="14">
+        <f t="shared" si="0"/>
+        <v>1.1416861826697891</v>
+      </c>
+      <c r="K54" s="14"/>
+      <c r="L54" s="14"/>
+      <c r="N54" s="18">
         <f t="shared" si="1"/>
-        <v>195</v>
-      </c>
-      <c r="L54" s="14">
-        <f t="shared" si="4"/>
-        <v>156</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.91334894613583129</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>40664</v>
       </c>
@@ -11862,19 +11760,17 @@
         <v>2507323.0970000001</v>
       </c>
       <c r="J55" s="14">
-        <f t="shared" si="3"/>
-        <v>1.0429252782193958</v>
-      </c>
-      <c r="K55" s="14">
+        <f t="shared" si="0"/>
+        <v>1.166429587482219</v>
+      </c>
+      <c r="K55" s="14"/>
+      <c r="L55" s="14"/>
+      <c r="N55" s="18">
         <f t="shared" si="1"/>
-        <v>205</v>
-      </c>
-      <c r="L55" s="14">
-        <f>K55*0.8</f>
-        <v>164</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.93314366998577525</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
         <v>40695</v>
       </c>
@@ -11900,19 +11796,17 @@
         <v>2517929.5669999998</v>
       </c>
       <c r="J56" s="14">
-        <f t="shared" si="3"/>
-        <v>1.0023419203747073</v>
-      </c>
-      <c r="K56" s="14">
+        <f t="shared" si="0"/>
+        <v>1.1073738680465719</v>
+      </c>
+      <c r="K56" s="14"/>
+      <c r="L56" s="14"/>
+      <c r="N56" s="18">
         <f t="shared" si="1"/>
-        <v>214</v>
-      </c>
-      <c r="L56" s="14">
-        <f t="shared" si="4"/>
-        <v>171.20000000000002</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.88589909443725756</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <v>40725</v>
       </c>
@@ -11938,19 +11832,17 @@
         <v>2664878.2579999999</v>
       </c>
       <c r="J57" s="14">
-        <f t="shared" si="3"/>
-        <v>1.0105263157894737</v>
-      </c>
-      <c r="K57" s="14">
+        <f t="shared" si="0"/>
+        <v>1.0990099009900991</v>
+      </c>
+      <c r="K57" s="14"/>
+      <c r="L57" s="14"/>
+      <c r="N57" s="18">
         <f t="shared" si="1"/>
-        <v>222</v>
-      </c>
-      <c r="L57" s="14">
-        <f t="shared" si="4"/>
-        <v>177.60000000000002</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.87920792079207932</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <v>40756</v>
       </c>
@@ -11976,19 +11868,17 @@
         <v>2828868.8390000002</v>
       </c>
       <c r="J58" s="14">
-        <f t="shared" si="3"/>
-        <v>0.96041397153945673</v>
-      </c>
-      <c r="K58" s="14">
+        <f t="shared" si="0"/>
+        <v>1.014207650273224</v>
+      </c>
+      <c r="K58" s="14"/>
+      <c r="L58" s="14"/>
+      <c r="N58" s="18">
         <f t="shared" si="1"/>
-        <v>232</v>
-      </c>
-      <c r="L58" s="14">
-        <f t="shared" si="4"/>
-        <v>185.60000000000002</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.81136612021857923</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>40787</v>
       </c>
@@ -12014,19 +11904,17 @@
         <v>3028610.3670000001</v>
       </c>
       <c r="J59" s="14">
-        <f t="shared" si="3"/>
-        <v>0.95445544554455453</v>
-      </c>
-      <c r="K59" s="14">
+        <f t="shared" si="0"/>
+        <v>0.99504541701073501</v>
+      </c>
+      <c r="K59" s="14"/>
+      <c r="L59" s="14"/>
+      <c r="N59" s="18">
         <f t="shared" si="1"/>
-        <v>241</v>
-      </c>
-      <c r="L59" s="14">
-        <f t="shared" si="4"/>
-        <v>192.8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.79603633360858805</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>40817</v>
       </c>
@@ -12052,19 +11940,17 @@
         <v>3074083.355</v>
       </c>
       <c r="J60" s="14">
-        <f t="shared" si="3"/>
-        <v>1.0754098360655737</v>
-      </c>
-      <c r="K60" s="14">
+        <f t="shared" si="0"/>
+        <v>1.0325288562434418</v>
+      </c>
+      <c r="K60" s="14"/>
+      <c r="L60" s="14"/>
+      <c r="N60" s="18">
         <f t="shared" si="1"/>
-        <v>246</v>
-      </c>
-      <c r="L60" s="14">
-        <f>K60</f>
-        <v>246</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.82602308499475352</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
         <v>40848</v>
       </c>
@@ -12090,19 +11976,17 @@
         <v>3251513.0329999998</v>
       </c>
       <c r="J61" s="14">
-        <f t="shared" si="3"/>
-        <v>1.036333608587944</v>
-      </c>
-      <c r="K61" s="14">
+        <f t="shared" si="0"/>
+        <v>1.0524109014675052</v>
+      </c>
+      <c r="K61" s="14"/>
+      <c r="L61" s="14"/>
+      <c r="N61" s="18">
         <f t="shared" si="1"/>
-        <v>251</v>
-      </c>
-      <c r="L61" s="14">
-        <f t="shared" ref="L61:L69" si="5">K61</f>
-        <v>251</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.84192872117400419</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
         <v>40878</v>
       </c>
@@ -12128,19 +12012,17 @@
         <v>3404973.6770000001</v>
       </c>
       <c r="J62" s="14">
-        <f t="shared" si="3"/>
-        <v>1.0786988457502624</v>
-      </c>
-      <c r="K62" s="14">
+        <f t="shared" si="0"/>
+        <v>1.0455655004068347</v>
+      </c>
+      <c r="K62" s="14"/>
+      <c r="L62" s="14"/>
+      <c r="N62" s="18">
         <f t="shared" si="1"/>
-        <v>257</v>
-      </c>
-      <c r="L62" s="14">
-        <f t="shared" si="5"/>
-        <v>257</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.83645240032546786</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>40909</v>
       </c>
@@ -12166,19 +12048,17 @@
         <v>3502929.5159999998</v>
       </c>
       <c r="J63" s="14">
-        <f t="shared" si="3"/>
-        <v>1.1069182389937107</v>
-      </c>
-      <c r="K63" s="14">
+        <f t="shared" si="0"/>
+        <v>1.0517928286852589</v>
+      </c>
+      <c r="K63" s="14"/>
+      <c r="L63" s="14"/>
+      <c r="N63" s="18">
         <f t="shared" si="1"/>
-        <v>264</v>
-      </c>
-      <c r="L63" s="14">
-        <f t="shared" si="5"/>
-        <v>264</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.84143426294820722</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
         <v>40940</v>
       </c>
@@ -12204,19 +12084,17 @@
         <v>3528982.8620000002</v>
       </c>
       <c r="J64" s="14">
-        <f t="shared" si="3"/>
-        <v>1.1065907241659885</v>
-      </c>
-      <c r="K64" s="14">
+        <f t="shared" si="0"/>
+        <v>1.0923694779116466</v>
+      </c>
+      <c r="K64" s="14"/>
+      <c r="L64" s="14"/>
+      <c r="N64" s="18">
         <f t="shared" si="1"/>
-        <v>272</v>
-      </c>
-      <c r="L64" s="14">
-        <f t="shared" si="5"/>
-        <v>272</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.8738955823293173</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <v>40969</v>
       </c>
@@ -12242,19 +12120,17 @@
         <v>3592352.0320000001</v>
       </c>
       <c r="J65" s="14">
-        <f t="shared" si="3"/>
-        <v>1.1155378486055776</v>
-      </c>
-      <c r="K65" s="14">
+        <f t="shared" si="0"/>
+        <v>1.0550113036925397</v>
+      </c>
+      <c r="K65" s="14"/>
+      <c r="L65" s="14"/>
+      <c r="N65" s="18">
         <f t="shared" si="1"/>
-        <v>280</v>
-      </c>
-      <c r="L65" s="14">
-        <f t="shared" si="5"/>
-        <v>280</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.84400904295403179</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
         <v>41000</v>
       </c>
@@ -12280,19 +12156,17 @@
         <v>3610648.2</v>
       </c>
       <c r="J66" s="14">
-        <f t="shared" si="3"/>
-        <v>1.1526104417670682</v>
-      </c>
-      <c r="K66" s="14">
+        <f t="shared" si="0"/>
+        <v>1.0669144981412639</v>
+      </c>
+      <c r="K66" s="14"/>
+      <c r="L66" s="14"/>
+      <c r="N66" s="18">
         <f t="shared" si="1"/>
-        <v>287</v>
-      </c>
-      <c r="L66" s="14">
-        <f t="shared" si="5"/>
-        <v>287</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.85353159851301119</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>41030</v>
       </c>
@@ -12318,19 +12192,17 @@
         <v>3775941.9029999999</v>
       </c>
       <c r="J67" s="14">
-        <f t="shared" si="3"/>
-        <v>1.1115297663903543</v>
-      </c>
-      <c r="K67" s="14">
+        <f t="shared" si="0"/>
+        <v>1.0592459605026929</v>
+      </c>
+      <c r="K67" s="14"/>
+      <c r="L67" s="14"/>
+      <c r="N67" s="18">
         <f t="shared" si="1"/>
-        <v>295</v>
-      </c>
-      <c r="L67" s="14">
-        <f t="shared" si="5"/>
-        <v>295</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.84739676840215439</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
         <v>41061</v>
       </c>
@@ -12356,19 +12228,17 @@
         <v>3870326.267</v>
       </c>
       <c r="J68" s="14">
-        <f t="shared" si="3"/>
-        <v>1.1301115241635689</v>
-      </c>
-      <c r="K68" s="14">
-        <f t="shared" ref="K68:K106" si="6">C68</f>
-        <v>304</v>
-      </c>
-      <c r="L68" s="14">
-        <f t="shared" si="5"/>
-        <v>304</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ref="J68:J106" si="2">C68/B68</f>
+        <v>1.1111111111111109</v>
+      </c>
+      <c r="K68" s="14"/>
+      <c r="L68" s="14"/>
+      <c r="N68" s="18">
+        <f t="shared" ref="N68:N106" si="3">J68*0.8</f>
+        <v>0.88888888888888884</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="7">
         <v>41091</v>
       </c>
@@ -12394,19 +12264,17 @@
         <v>3941389.5809999998</v>
       </c>
       <c r="J69" s="14">
+        <f t="shared" si="2"/>
+        <v>1.1692876965772432</v>
+      </c>
+      <c r="K69" s="14"/>
+      <c r="L69" s="14"/>
+      <c r="N69" s="18">
         <f t="shared" si="3"/>
-        <v>1.1346499102333931</v>
-      </c>
-      <c r="K69" s="14">
-        <f t="shared" si="6"/>
-        <v>316</v>
-      </c>
-      <c r="L69" s="14">
-        <f t="shared" si="5"/>
-        <v>316</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.93543015726179457</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
         <v>41122</v>
       </c>
@@ -12432,19 +12300,17 @@
         <v>4115200.4190000002</v>
       </c>
       <c r="J70" s="14">
+        <f t="shared" si="2"/>
+        <v>1.2285287528005975</v>
+      </c>
+      <c r="K70" s="14"/>
+      <c r="L70" s="14"/>
+      <c r="N70" s="18">
         <f t="shared" si="3"/>
-        <v>1.322733918128655</v>
-      </c>
-      <c r="K70" s="14">
-        <f t="shared" si="6"/>
-        <v>329</v>
-      </c>
-      <c r="L70" s="14">
-        <f>K70*1.1</f>
-        <v>361.90000000000003</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.98282300224047803</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="7">
         <v>41153</v>
       </c>
@@ -12470,19 +12336,17 @@
         <v>4235447.6670000004</v>
       </c>
       <c r="J71" s="14">
+        <f t="shared" si="2"/>
+        <v>1.2964728312678742</v>
+      </c>
+      <c r="K71" s="14"/>
+      <c r="L71" s="14"/>
+      <c r="N71" s="18">
         <f t="shared" si="3"/>
-        <v>1.3839037927844591</v>
-      </c>
-      <c r="K71" s="14">
-        <f t="shared" si="6"/>
-        <v>340</v>
-      </c>
-      <c r="L71" s="14">
-        <f t="shared" ref="L71:L81" si="7">K71*1.1</f>
-        <v>374.00000000000006</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.0371782650142993</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
         <v>41183</v>
       </c>
@@ -12508,19 +12372,17 @@
         <v>4325251.7740000002</v>
       </c>
       <c r="J72" s="14">
+        <f t="shared" si="2"/>
+        <v>1.3423076923076922</v>
+      </c>
+      <c r="K72" s="14"/>
+      <c r="L72" s="14"/>
+      <c r="N72" s="18">
         <f t="shared" si="3"/>
-        <v>1.4335324869305452</v>
-      </c>
-      <c r="K72" s="14">
-        <f t="shared" si="6"/>
-        <v>349</v>
-      </c>
-      <c r="L72" s="14">
-        <f t="shared" si="7"/>
-        <v>383.90000000000003</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.0738461538461539</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
         <v>41214</v>
       </c>
@@ -12546,19 +12408,17 @@
         <v>4488731.767</v>
       </c>
       <c r="J73" s="14">
-        <f t="shared" ref="J73:J106" si="8">L73/B71</f>
-        <v>1.501620591039085</v>
-      </c>
-      <c r="K73" s="14">
-        <f t="shared" si="6"/>
-        <v>358</v>
-      </c>
-      <c r="L73" s="14">
-        <f t="shared" si="7"/>
-        <v>393.8</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.3801079414032384</v>
+      </c>
+      <c r="K73" s="14"/>
+      <c r="L73" s="14"/>
+      <c r="N73" s="18">
+        <f t="shared" si="3"/>
+        <v>1.1040863531225908</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="7">
         <v>41244</v>
       </c>
@@ -12584,19 +12444,17 @@
         <v>4484293.2580000004</v>
       </c>
       <c r="J74" s="14">
-        <f t="shared" si="8"/>
-        <v>1.5653846153846156</v>
-      </c>
-      <c r="K74" s="14">
-        <f t="shared" si="6"/>
-        <v>370</v>
-      </c>
-      <c r="L74" s="14">
-        <f t="shared" si="7"/>
-        <v>407.00000000000006</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.4176245210727969</v>
+      </c>
+      <c r="K74" s="14"/>
+      <c r="L74" s="14"/>
+      <c r="N74" s="18">
+        <f t="shared" si="3"/>
+        <v>1.1340996168582376</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="7">
         <v>41275</v>
       </c>
@@ -12622,19 +12480,17 @@
         <v>4573242.5159999998</v>
       </c>
       <c r="J75" s="14">
-        <f t="shared" si="8"/>
-        <v>1.6410948342328453</v>
-      </c>
-      <c r="K75" s="14">
-        <f t="shared" si="6"/>
-        <v>387</v>
-      </c>
-      <c r="L75" s="14">
-        <f t="shared" si="7"/>
-        <v>425.70000000000005</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
+      <c r="K75" s="14"/>
+      <c r="L75" s="14"/>
+      <c r="N75" s="18">
+        <f t="shared" si="3"/>
+        <v>1.2000000000000002</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="7">
         <v>41306</v>
       </c>
@@ -12660,19 +12516,17 @@
         <v>4834129.7139999997</v>
       </c>
       <c r="J76" s="14">
-        <f t="shared" si="8"/>
-        <v>1.7153256704980844</v>
-      </c>
-      <c r="K76" s="14">
-        <f t="shared" si="6"/>
-        <v>407</v>
-      </c>
-      <c r="L76" s="14">
-        <f t="shared" si="7"/>
-        <v>447.70000000000005</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.5759922555663117</v>
+      </c>
+      <c r="K76" s="14"/>
+      <c r="L76" s="14"/>
+      <c r="N76" s="18">
+        <f t="shared" si="3"/>
+        <v>1.2607938044530496</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="7">
         <v>41334</v>
       </c>
@@ -12698,19 +12552,17 @@
         <v>5002855</v>
       </c>
       <c r="J77" s="14">
-        <f t="shared" si="8"/>
-        <v>1.816279069767442</v>
-      </c>
-      <c r="K77" s="14">
-        <f t="shared" si="6"/>
-        <v>426</v>
-      </c>
-      <c r="L77" s="14">
-        <f t="shared" si="7"/>
-        <v>468.6</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.6999201915403033</v>
+      </c>
+      <c r="K77" s="14"/>
+      <c r="L77" s="14"/>
+      <c r="N77" s="18">
+        <f t="shared" si="3"/>
+        <v>1.3599361532322427</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="7">
         <v>41365</v>
       </c>
@@ -12736,19 +12588,17 @@
         <v>5089761.5329999998</v>
       </c>
       <c r="J78" s="14">
-        <f t="shared" si="8"/>
-        <v>1.8954501452081318</v>
-      </c>
-      <c r="K78" s="14">
-        <f t="shared" si="6"/>
-        <v>445</v>
-      </c>
-      <c r="L78" s="14">
-        <f t="shared" si="7"/>
-        <v>489.50000000000006</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.733203505355404</v>
+      </c>
+      <c r="K78" s="14"/>
+      <c r="L78" s="14"/>
+      <c r="N78" s="18">
+        <f t="shared" si="3"/>
+        <v>1.3865628042843232</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="7">
         <v>41395</v>
       </c>
@@ -12774,19 +12624,17 @@
         <v>5278897.3870000001</v>
       </c>
       <c r="J79" s="14">
-        <f t="shared" si="8"/>
-        <v>2.0147645650438948</v>
-      </c>
-      <c r="K79" s="14">
-        <f t="shared" si="6"/>
-        <v>459</v>
-      </c>
-      <c r="L79" s="14">
-        <f t="shared" si="7"/>
-        <v>504.90000000000003</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.7804499612102405</v>
+      </c>
+      <c r="K79" s="14"/>
+      <c r="L79" s="14"/>
+      <c r="N79" s="18">
+        <f t="shared" si="3"/>
+        <v>1.4243599689681925</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="7">
         <v>41426</v>
       </c>
@@ -12812,19 +12660,17 @@
         <v>5434795.0999999996</v>
       </c>
       <c r="J80" s="14">
-        <f t="shared" si="8"/>
-        <v>2.0179162609542356</v>
-      </c>
-      <c r="K80" s="14">
-        <f t="shared" si="6"/>
-        <v>471</v>
-      </c>
-      <c r="L80" s="14">
-        <f t="shared" si="7"/>
-        <v>518.1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.8727634194831013</v>
+      </c>
+      <c r="K80" s="14"/>
+      <c r="L80" s="14"/>
+      <c r="N80" s="18">
+        <f t="shared" si="3"/>
+        <v>1.4982107355864811</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="7">
         <v>41456</v>
       </c>
@@ -12850,19 +12696,17 @@
         <v>5481862.5810000002</v>
       </c>
       <c r="J81" s="14">
-        <f t="shared" si="8"/>
-        <v>2.0523661753297131</v>
-      </c>
-      <c r="K81" s="14">
-        <f t="shared" si="6"/>
-        <v>481</v>
-      </c>
-      <c r="L81" s="14">
-        <f t="shared" si="7"/>
-        <v>529.1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.8734177215189873</v>
+      </c>
+      <c r="K81" s="14"/>
+      <c r="L81" s="14"/>
+      <c r="N81" s="18">
+        <f t="shared" si="3"/>
+        <v>1.4987341772151899</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="7">
         <v>41487</v>
       </c>
@@ -12888,19 +12732,17 @@
         <v>5467691.71</v>
       </c>
       <c r="J82" s="14">
-        <f t="shared" si="8"/>
-        <v>1.9602385685884691</v>
-      </c>
-      <c r="K82" s="14">
-        <f t="shared" si="6"/>
-        <v>493</v>
-      </c>
-      <c r="L82" s="14">
-        <f>K82</f>
-        <v>493</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.8990755007704159</v>
+      </c>
+      <c r="K82" s="14"/>
+      <c r="L82" s="14"/>
+      <c r="N82" s="18">
+        <f t="shared" si="3"/>
+        <v>1.5192604006163328</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="7">
         <v>41518</v>
       </c>
@@ -12926,19 +12768,17 @@
         <v>5542970.0999999996</v>
       </c>
       <c r="J83" s="14">
-        <f t="shared" si="8"/>
-        <v>1.9513145082765335</v>
-      </c>
-      <c r="K83" s="14">
-        <f t="shared" si="6"/>
-        <v>501</v>
-      </c>
-      <c r="L83" s="14">
-        <f t="shared" ref="L83:L90" si="9">K83</f>
-        <v>501</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.9195402298850575</v>
+      </c>
+      <c r="K83" s="14"/>
+      <c r="L83" s="14"/>
+      <c r="N83" s="18">
+        <f t="shared" si="3"/>
+        <v>1.535632183908046</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="7">
         <v>41548</v>
       </c>
@@ -12964,19 +12804,17 @@
         <v>5466187.3229999999</v>
       </c>
       <c r="J84" s="14">
-        <f t="shared" si="8"/>
-        <v>1.9453004622496146</v>
-      </c>
-      <c r="K84" s="14">
-        <f t="shared" si="6"/>
-        <v>505</v>
-      </c>
-      <c r="L84" s="14">
-        <f t="shared" si="9"/>
-        <v>505</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.9940769990128331</v>
+      </c>
+      <c r="K84" s="14"/>
+      <c r="L84" s="14"/>
+      <c r="N84" s="18">
+        <f t="shared" si="3"/>
+        <v>1.5952615992102666</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="7">
         <v>41579</v>
       </c>
@@ -13002,19 +12840,17 @@
         <v>5439027.8329999996</v>
       </c>
       <c r="J85" s="14">
-        <f t="shared" si="8"/>
-        <v>1.9425287356321839</v>
-      </c>
-      <c r="K85" s="14">
-        <f t="shared" si="6"/>
-        <v>507</v>
-      </c>
-      <c r="L85" s="14">
-        <f t="shared" si="9"/>
-        <v>507</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.983568075117371</v>
+      </c>
+      <c r="K85" s="14"/>
+      <c r="L85" s="14"/>
+      <c r="N85" s="18">
+        <f t="shared" si="3"/>
+        <v>1.586854460093897</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="7">
         <v>41609</v>
       </c>
@@ -13040,19 +12876,17 @@
         <v>5668821.29</v>
       </c>
       <c r="J86" s="14">
-        <f t="shared" si="8"/>
-        <v>2.0138203356367228</v>
-      </c>
-      <c r="K86" s="14">
-        <f t="shared" si="6"/>
-        <v>510</v>
-      </c>
-      <c r="L86" s="14">
-        <f t="shared" si="9"/>
-        <v>510</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.9484240687679084</v>
+      </c>
+      <c r="K86" s="14"/>
+      <c r="L86" s="14"/>
+      <c r="N86" s="18">
+        <f t="shared" si="3"/>
+        <v>1.5587392550143269</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="7">
         <v>41640</v>
       </c>
@@ -13078,19 +12912,17 @@
         <v>5684717.0650000004</v>
       </c>
       <c r="J87" s="14">
-        <f t="shared" si="8"/>
-        <v>2.0266040688575901</v>
-      </c>
-      <c r="K87" s="14">
-        <f t="shared" si="6"/>
-        <v>518</v>
-      </c>
-      <c r="L87" s="14">
-        <f t="shared" si="9"/>
-        <v>518</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.9923076923076923</v>
+      </c>
+      <c r="K87" s="14"/>
+      <c r="L87" s="14"/>
+      <c r="N87" s="18">
+        <f t="shared" si="3"/>
+        <v>1.5938461538461539</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="7">
         <v>41671</v>
       </c>
@@ -13116,19 +12948,17 @@
         <v>5780611.4639999997</v>
       </c>
       <c r="J88" s="14">
-        <f t="shared" si="8"/>
-        <v>2.0248328557784143</v>
-      </c>
-      <c r="K88" s="14">
-        <f t="shared" si="6"/>
-        <v>530</v>
-      </c>
-      <c r="L88" s="14">
-        <f t="shared" si="9"/>
-        <v>530</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>2.052274927395934</v>
+      </c>
+      <c r="K88" s="14"/>
+      <c r="L88" s="14"/>
+      <c r="N88" s="18">
+        <f t="shared" si="3"/>
+        <v>1.6418199419167472</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="7">
         <v>41699</v>
       </c>
@@ -13154,19 +12984,17 @@
         <v>5958706.0319999997</v>
       </c>
       <c r="J89" s="14">
-        <f t="shared" si="8"/>
-        <v>2.0846153846153848</v>
-      </c>
-      <c r="K89" s="14">
-        <f t="shared" si="6"/>
-        <v>542</v>
-      </c>
-      <c r="L89" s="14">
-        <f t="shared" si="9"/>
-        <v>542</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>2.0786193672099711</v>
+      </c>
+      <c r="K89" s="14"/>
+      <c r="L89" s="14"/>
+      <c r="N89" s="18">
+        <f t="shared" si="3"/>
+        <v>1.662895493767977</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="7">
         <v>41730</v>
       </c>
@@ -13192,19 +13020,17 @@
         <v>6222101.7999999998</v>
       </c>
       <c r="J90" s="14">
-        <f t="shared" si="8"/>
-        <v>2.1335914811229428</v>
-      </c>
-      <c r="K90" s="14">
-        <f t="shared" si="6"/>
-        <v>551</v>
-      </c>
-      <c r="L90" s="14">
-        <f t="shared" si="9"/>
-        <v>551</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>2.1090909090909089</v>
+      </c>
+      <c r="K90" s="14"/>
+      <c r="L90" s="14"/>
+      <c r="N90" s="18">
+        <f t="shared" si="3"/>
+        <v>1.6872727272727273</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="7">
         <v>41760</v>
       </c>
@@ -13230,19 +13056,17 @@
         <v>6364343.4840000002</v>
       </c>
       <c r="J91" s="14">
-        <f t="shared" si="8"/>
-        <v>2.0038350910834133</v>
-      </c>
-      <c r="K91" s="14">
-        <f t="shared" si="6"/>
-        <v>555</v>
-      </c>
-      <c r="L91" s="14">
-        <f>B90*2</f>
-        <v>522.5</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>2.1379044684129429</v>
+      </c>
+      <c r="K91" s="14"/>
+      <c r="L91" s="14"/>
+      <c r="N91" s="18">
+        <f t="shared" si="3"/>
+        <v>1.7103235747303545</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="7">
         <v>41791</v>
       </c>
@@ -13268,19 +13092,17 @@
         <v>6522072.2999999998</v>
       </c>
       <c r="J92" s="14">
-        <f t="shared" si="8"/>
-        <v>1.9873684210526317</v>
-      </c>
-      <c r="K92" s="14">
-        <f t="shared" si="6"/>
-        <v>558</v>
-      </c>
-      <c r="L92" s="14">
-        <f t="shared" ref="L92:L106" si="10">B91*2</f>
-        <v>519.20000000000005</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>2.1399808245445828</v>
+      </c>
+      <c r="K92" s="14"/>
+      <c r="L92" s="14"/>
+      <c r="N92" s="18">
+        <f t="shared" si="3"/>
+        <v>1.7119846596356663</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="7">
         <v>41821</v>
       </c>
@@ -13306,19 +13128,17 @@
         <v>6522273.8059999999</v>
       </c>
       <c r="J93" s="14">
-        <f t="shared" si="8"/>
-        <v>2.008859784283513</v>
-      </c>
-      <c r="K93" s="14">
-        <f t="shared" si="6"/>
-        <v>560</v>
-      </c>
-      <c r="L93" s="14">
-        <f t="shared" si="10"/>
-        <v>521.5</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>2.1435406698564594</v>
+      </c>
+      <c r="K93" s="14"/>
+      <c r="L93" s="14"/>
+      <c r="N93" s="18">
+        <f t="shared" si="3"/>
+        <v>1.7148325358851677</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="7">
         <v>41852</v>
       </c>
@@ -13344,19 +13164,17 @@
         <v>6580583.3229999999</v>
       </c>
       <c r="J94" s="14">
-        <f t="shared" si="8"/>
-        <v>2.0038350910834133</v>
-      </c>
-      <c r="K94" s="14">
-        <f t="shared" si="6"/>
-        <v>564</v>
-      </c>
-      <c r="L94" s="14">
-        <f t="shared" si="10"/>
-        <v>522.5</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>2.2065727699530515</v>
+      </c>
+      <c r="K94" s="14"/>
+      <c r="L94" s="14"/>
+      <c r="N94" s="18">
+        <f t="shared" si="3"/>
+        <v>1.7652582159624413</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="7">
         <v>41883</v>
       </c>
@@ -13382,19 +13200,17 @@
         <v>6557719.3669999996</v>
       </c>
       <c r="J95" s="14">
-        <f t="shared" si="8"/>
-        <v>1.9567464114832536</v>
-      </c>
-      <c r="K95" s="14">
-        <f t="shared" si="6"/>
-        <v>565</v>
-      </c>
-      <c r="L95" s="14">
-        <f t="shared" si="10"/>
-        <v>511.2</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>2.202729044834308</v>
+      </c>
+      <c r="K95" s="14"/>
+      <c r="L95" s="14"/>
+      <c r="N95" s="18">
+        <f t="shared" si="3"/>
+        <v>1.7621832358674465</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="7">
         <v>41913</v>
       </c>
@@ -13420,19 +13236,17 @@
         <v>6650755.6129999999</v>
       </c>
       <c r="J96" s="14">
-        <f t="shared" si="8"/>
-        <v>2.007042253521127</v>
-      </c>
-      <c r="K96" s="14">
-        <f t="shared" si="6"/>
-        <v>566</v>
-      </c>
-      <c r="L96" s="14">
-        <f t="shared" si="10"/>
-        <v>513</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>2.1087928464977646</v>
+      </c>
+      <c r="K96" s="14"/>
+      <c r="L96" s="14"/>
+      <c r="N96" s="18">
+        <f t="shared" si="3"/>
+        <v>1.6870342771982116</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="7">
         <v>41944</v>
       </c>
@@ -13458,19 +13272,17 @@
         <v>6752266.1330000004</v>
       </c>
       <c r="J97" s="14">
-        <f t="shared" si="8"/>
-        <v>2.0927875243664715</v>
-      </c>
-      <c r="K97" s="14">
-        <f t="shared" si="6"/>
-        <v>583</v>
-      </c>
-      <c r="L97" s="14">
-        <f t="shared" si="10"/>
-        <v>536.79999999999995</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>2.2125237191650853</v>
+      </c>
+      <c r="K97" s="14"/>
+      <c r="L97" s="14"/>
+      <c r="N97" s="18">
+        <f t="shared" si="3"/>
+        <v>1.7700189753320683</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="7">
         <v>41974</v>
       </c>
@@ -13496,19 +13308,17 @@
         <v>7107867.8710000003</v>
       </c>
       <c r="J98" s="14">
-        <f t="shared" si="8"/>
-        <v>1.9634873323397914</v>
-      </c>
-      <c r="K98" s="14">
-        <f t="shared" si="6"/>
-        <v>601</v>
-      </c>
-      <c r="L98" s="14">
-        <f t="shared" si="10"/>
-        <v>527</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>2.3453658536585364</v>
+      </c>
+      <c r="K98" s="14"/>
+      <c r="L98" s="14"/>
+      <c r="N98" s="18">
+        <f t="shared" si="3"/>
+        <v>1.8762926829268292</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="7">
         <v>42005</v>
       </c>
@@ -13534,19 +13344,17 @@
         <v>7058875.5159999998</v>
       </c>
       <c r="J99" s="14">
-        <f t="shared" si="8"/>
-        <v>1.9449715370018976</v>
-      </c>
-      <c r="K99" s="14">
-        <f t="shared" si="6"/>
-        <v>619</v>
-      </c>
-      <c r="L99" s="14">
-        <f t="shared" si="10"/>
-        <v>512.5</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>2.6385336743393011</v>
+      </c>
+      <c r="K99" s="14"/>
+      <c r="L99" s="14"/>
+      <c r="N99" s="18">
+        <f t="shared" si="3"/>
+        <v>2.110826939471441</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="7">
         <v>42036</v>
       </c>
@@ -13572,19 +13380,17 @@
         <v>7288602.1789999995</v>
       </c>
       <c r="J100" s="14">
-        <f t="shared" si="8"/>
-        <v>1.8310243902439023</v>
-      </c>
-      <c r="K100" s="14">
-        <f t="shared" si="6"/>
-        <v>638</v>
-      </c>
-      <c r="L100" s="14">
-        <f t="shared" si="10"/>
-        <v>469.2</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>3.3229166666666665</v>
+      </c>
+      <c r="K100" s="14"/>
+      <c r="L100" s="14"/>
+      <c r="N100" s="18">
+        <f t="shared" si="3"/>
+        <v>2.6583333333333332</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="7">
         <v>42064</v>
       </c>
@@ -13610,19 +13416,17 @@
         <v>7306929.9680000003</v>
       </c>
       <c r="J101" s="14">
-        <f t="shared" si="8"/>
-        <v>1.6368286445012787</v>
-      </c>
-      <c r="K101" s="14">
-        <f t="shared" si="6"/>
-        <v>655</v>
-      </c>
-      <c r="L101" s="14">
-        <f t="shared" si="10"/>
-        <v>384</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>4.1653418124006363</v>
+      </c>
+      <c r="K101" s="14"/>
+      <c r="L101" s="14"/>
+      <c r="N101" s="18">
+        <f t="shared" si="3"/>
+        <v>3.3322734499205091</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="7">
         <v>42095</v>
       </c>
@@ -13648,19 +13452,17 @@
         <v>7341966.7769999998</v>
       </c>
       <c r="J102" s="14">
-        <f t="shared" si="8"/>
-        <v>1.6380208333333333</v>
-      </c>
-      <c r="K102" s="14">
-        <f t="shared" si="6"/>
-        <v>675</v>
-      </c>
-      <c r="L102" s="14">
-        <f t="shared" si="10"/>
-        <v>314.5</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>4.9270072992700733</v>
+      </c>
+      <c r="K102" s="14"/>
+      <c r="L102" s="14"/>
+      <c r="N102" s="18">
+        <f t="shared" si="3"/>
+        <v>3.9416058394160589</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="7">
         <v>42125</v>
       </c>
@@ -13686,19 +13488,17 @@
         <v>7313457.1160000004</v>
       </c>
       <c r="J103" s="14">
-        <f t="shared" si="8"/>
-        <v>1.7424483306836247</v>
-      </c>
-      <c r="K103" s="14">
-        <f t="shared" si="6"/>
-        <v>697</v>
-      </c>
-      <c r="L103" s="14">
-        <f t="shared" si="10"/>
-        <v>274</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>5.7413509060955512</v>
+      </c>
+      <c r="K103" s="14"/>
+      <c r="L103" s="14"/>
+      <c r="N103" s="18">
+        <f t="shared" si="3"/>
+        <v>4.5930807248764411</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" s="7">
         <v>42156</v>
       </c>
@@ -13724,19 +13524,17 @@
         <v>7247929.4929999998</v>
       </c>
       <c r="J104" s="14">
-        <f t="shared" si="8"/>
-        <v>1.7722627737226277</v>
-      </c>
-      <c r="K104" s="14">
-        <f t="shared" si="6"/>
-        <v>720</v>
-      </c>
-      <c r="L104" s="14">
-        <f t="shared" si="10"/>
-        <v>242.8</v>
-      </c>
-    </row>
-    <row r="105" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>6.4429530201342278</v>
+      </c>
+      <c r="K104" s="14"/>
+      <c r="L104" s="14"/>
+      <c r="N104" s="18">
+        <f t="shared" si="3"/>
+        <v>5.1543624161073822</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="7">
         <v>42186</v>
       </c>
@@ -13762,19 +13560,17 @@
         <v>7153020.3810000001</v>
       </c>
       <c r="J105" s="14">
-        <f t="shared" si="8"/>
-        <v>1.8410214168039538</v>
-      </c>
-      <c r="K105" s="14">
-        <f t="shared" si="6"/>
-        <v>743</v>
-      </c>
-      <c r="L105" s="14">
-        <f t="shared" si="10"/>
-        <v>223.5</v>
-      </c>
-    </row>
-    <row r="106" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>6.7668488160291442</v>
+      </c>
+      <c r="K105" s="14"/>
+      <c r="L105" s="14"/>
+      <c r="N105" s="18">
+        <f t="shared" si="3"/>
+        <v>5.4134790528233161</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="7">
         <v>42217</v>
       </c>
@@ -13800,19 +13596,17 @@
         <v>7039996.5089999996</v>
       </c>
       <c r="J106" s="14">
-        <f>L106/B104</f>
-        <v>1.9651006711409396</v>
-      </c>
-      <c r="K106" s="14">
-        <f t="shared" si="6"/>
-        <v>767</v>
-      </c>
-      <c r="L106" s="14">
-        <f t="shared" si="10"/>
-        <v>219.6</v>
-      </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>7.0854503464203233</v>
+      </c>
+      <c r="K106" s="14"/>
+      <c r="L106" s="14"/>
+      <c r="N106" s="18">
+        <f t="shared" si="3"/>
+        <v>5.6683602771362587</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" s="7">
         <v>42248</v>
       </c>
@@ -13838,7 +13632,7 @@
       <c r="J107" s="15"/>
       <c r="K107" s="14"/>
     </row>
-    <row r="108" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="7">
         <v>42278</v>
       </c>

</xml_diff>